<commit_message>
commit jeep notebook and dataframe updated
</commit_message>
<xml_diff>
--- a/dataframe_each_make_xlsx_file/df_jeep_updated.xlsx
+++ b/dataframe_each_make_xlsx_file/df_jeep_updated.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,7 +577,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -586,7 +586,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Cherokee</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -605,7 +605,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>2007</v>
+        <v>1999</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -614,12 +614,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Grand Cherokee Overland</t>
+          <t>Grand Cherokee Laredo</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Opt</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -633,7 +633,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>2007</v>
+        <v>1999</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -642,12 +642,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Commander</t>
+          <t>Wrangler</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Opt</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -661,7 +661,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2007</v>
+        <v>1999</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -670,7 +670,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Patriot</t>
+          <t>Grand Cherokee Limited</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -689,26 +689,2518 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Cherokee</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Opt</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Opt</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Cherokee</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Opt</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Opt</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2002</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Opt</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2002</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Opt (Std on Sahara)</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2002</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2002</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2003</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Opt</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2003</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Opt (Std on Sahara)</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2003</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2003</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2004</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Opt</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2004</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Opt (Std on Sahara)</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2004</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2004</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2005</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Opt</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2005</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2005</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
         <v>2007</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Jeep</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Overland</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Commander</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Patriot</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
         <is>
           <t>Compass</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>Std w/o  power windows &amp; power locks</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Std w/o power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Overland</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Commander</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Patriot</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Std w/o power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Std w/o power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2008</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Overland</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Commander</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Patriot</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Std w/o  power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Std w/o power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2009</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Overland</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Commander</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Patriot</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Std w/o  power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Std w/o power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Overland</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Patriot</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Std w/o  power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Std w/o power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Overland</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Patriot</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Std w/o  power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Std w/o power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>2012</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>- Std with power windows &amp; power locks ----</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Laredo</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Limited</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Grand Cherokee Overland</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Liberty</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Patriot</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Std</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Information not available</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Std w/o  power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Wrangler</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Std w/o power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Compass</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Std with power windows &amp; power locks</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
commit the df_jeep after modifications: change the models Compass and Wrangler
</commit_message>
<xml_diff>
--- a/dataframe_each_make_xlsx_file/df_jeep_updated.xlsx
+++ b/dataframe_each_make_xlsx_file/df_jeep_updated.xlsx
@@ -810,12 +810,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Cherokee</t>
+          <t>Grand Cherokee Limited</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Opt</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -838,12 +838,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Grand Cherokee Laredo</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Opt</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -866,12 +866,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Grand Cherokee Laredo</t>
+          <t>Cherokee</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Opt</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -894,12 +894,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Grand Cherokee Limited</t>
+          <t>Wrangler</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Opt</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1034,12 +1034,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Grand Cherokee Limited</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Opt</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1062,12 +1062,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Opt (Std on Sahara)</t>
+          <t>Opt</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1090,12 +1090,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Grand Cherokee Laredo</t>
+          <t>Wrangler</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Opt (Std on Sahara)</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Grand Cherokee Limited</t>
+          <t>Grand Cherokee Laredo</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1146,12 +1146,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Grand Cherokee Laredo</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Opt</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1174,12 +1174,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Grand Cherokee Limited</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Opt (Std on Sahara)</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1202,12 +1202,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Grand Cherokee Laredo</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Opt</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1230,12 +1230,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Grand Cherokee Limited</t>
+          <t>Wrangler</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t>Opt (Std on Sahara)</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Grand Cherokee Laredo</t>
+          <t>Compass (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1352,7 +1352,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -1370,7 +1370,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Grand Cherokee Limited</t>
+          <t>Wrangler (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Grand Cherokee Overland</t>
+          <t>Patriot</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1426,7 +1426,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Commander</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1454,7 +1454,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Wrangler (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Patriot</t>
+          <t>Grand Cherokee Overland</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1510,17 +1510,17 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Compass (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Std w/o  power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -1538,17 +1538,17 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Grand Cherokee Limited</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Std w/o power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Grand Cherokee Laredo</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -1594,17 +1594,17 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Commander</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -1622,7 +1622,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Grand Cherokee Laredo</t>
+          <t>Wrangler (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Grand Cherokee Limited</t>
+          <t>Compass (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -1678,7 +1678,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Grand Cherokee Overland</t>
+          <t>Compass (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Commander</t>
+          <t>Wrangler (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Patriot</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Patriot</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1790,17 +1790,17 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Grand Cherokee Overland</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Std w/o power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -1818,17 +1818,17 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Grand Cherokee Limited</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Std w/o power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -1846,17 +1846,17 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Grand Cherokee Laredo</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -1874,17 +1874,17 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Commander</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Grand Cherokee Laredo</t>
+          <t>Wrangler (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1912,7 +1912,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Grand Cherokee Limited</t>
+          <t>Compass (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1940,7 +1940,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -1958,7 +1958,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Grand Cherokee Overland</t>
+          <t>Wrangler (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Commander</t>
+          <t>Compass (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Patriot</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Patriot</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2070,17 +2070,17 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Grand Cherokee Laredo</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Std w/o  power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2098,17 +2098,17 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Grand Cherokee Limited</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Std w/o power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2126,17 +2126,17 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Grand Cherokee Overland</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2154,17 +2154,17 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Commander</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Grand Cherokee Laredo</t>
+          <t>Grand Cherokee Overland</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Grand Cherokee Limited</t>
+          <t>Commander</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Grand Cherokee Overland</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2266,7 +2266,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Commander</t>
+          <t>Patriot</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2294,7 +2294,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Wrangler (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2304,7 +2304,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Patriot</t>
+          <t>Compass (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2332,7 +2332,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -2350,17 +2350,17 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Grand Cherokee Limited</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Std w/o  power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2378,12 +2378,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Compass (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Std w/o power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -2406,17 +2406,17 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Wrangler (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -2434,17 +2434,17 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Grand Cherokee Laredo</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2462,7 +2462,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Grand Cherokee Laredo</t>
+          <t>Compass (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2472,7 +2472,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Grand Cherokee Limited</t>
+          <t>Grand Cherokee Laredo</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Grand Cherokee Overland</t>
+          <t>Compass (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2528,7 +2528,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -2546,7 +2546,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Wrangler (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Patriot</t>
+          <t>Wrangler (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2584,7 +2584,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -2602,17 +2602,17 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Grand Cherokee Limited</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Std w/o  power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2630,17 +2630,17 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Grand Cherokee Overland</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Std w/o power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2658,17 +2658,17 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2686,17 +2686,17 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Patriot</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Grand Cherokee Laredo</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2742,7 +2742,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Grand Cherokee Limited</t>
+          <t>Wrangler (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2752,7 +2752,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -2770,7 +2770,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Grand Cherokee Overland</t>
+          <t>Compass (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2780,7 +2780,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Compass (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2808,7 +2808,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Patriot</t>
+          <t>Wrangler (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -2854,17 +2854,17 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Grand Cherokee Laredo</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Std w/o  power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2882,17 +2882,17 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Patriot</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Std w/o power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2910,17 +2910,17 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Grand Cherokee Limited</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2938,17 +2938,17 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Grand Cherokee Overland</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -2966,17 +2966,17 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>- Std with power windows &amp; power locks ----</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Grand Cherokee Limited</t>
+          <t>Compass (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -3032,7 +3032,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Grand Cherokee Overland</t>
+          <t>Compass (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -3060,7 +3060,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -3078,17 +3078,17 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Liberty</t>
+          <t>Wrangler (W/ power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Std</t>
+          <t xml:space="preserve"> Std </t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Information not available</t>
+          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
         </is>
       </c>
     </row>
@@ -3106,7 +3106,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Patriot</t>
+          <t>Grand Cherokee Limited</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3134,17 +3134,17 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Grand Cherokee Overland</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Std w/o  power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -3162,17 +3162,17 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Wrangler</t>
+          <t>Patriot</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Std w/o power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Sentry Key Immobilizer System = Standard equipment</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -3190,17 +3190,17 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Compass</t>
+          <t>Wrangler (W/O power windows &amp; power locks)</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Std with power windows &amp; power locks</t>
+          <t>Std</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>“SKREES” Sentry Key Remote Entry System (same as SKIS, the key remote entry module was combined with the Sentry Key Immobilizer Module, it’s still Sentry Key)</t>
+          <t>Sentry Key Immobilizer System = Standard equipment</t>
         </is>
       </c>
     </row>

</xml_diff>